<commit_message>
Update cached files in C# Add description comment to Digitize,Clasify and Export test cases in VB and C#
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt1/CSharp/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt1/CSharp/Tests/Cache/Config_Expected.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.hojda\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt1\CSharp\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.hojda\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC960BA-D9DB-4236-A9EA-A6E74E80E0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65071DC9-9CC3-4E4E-B540-A91DCA7097C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -5067,8 +5067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5271,21 +5271,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E3A3D5-A5D2-470F-B877-63AC0F081528}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D1FA23-0F05-4B8D-B77D-DF9AB2091E72}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" customWidth="1"/>
-    <col min="2" max="2" width="73.42578125" customWidth="1"/>
-    <col min="3" max="3" width="114.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.28515625" customWidth="1"/>
+    <col min="2" max="2" width="79.42578125" customWidth="1"/>
+    <col min="3" max="3" width="221.28515625" customWidth="1"/>
+    <col min="4" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>